<commit_message>
implement JsonHPackProcessor & update benchmark results
</commit_message>
<xml_diff>
--- a/jsonBenchmark.xlsx
+++ b/jsonBenchmark.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Original JSON size (bytes)</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>Gzipped + Minimized</t>
-  </si>
-  <si>
-    <t>Gzipped + Compressed</t>
   </si>
   <si>
     <t>json1</t>
@@ -51,14 +48,29 @@
     <t>Original JSON size (%)</t>
   </si>
   <si>
-    <t>Diff Compressed vs Non Compressed</t>
+    <t>Compress cjson</t>
+  </si>
+  <si>
+    <t>Compress hpack</t>
+  </si>
+  <si>
+    <t>Gzipped + Compress hpack</t>
+  </si>
+  <si>
+    <t>Gzipped + Compress cjson</t>
+  </si>
+  <si>
+    <t>Diff Compres cjson vs Gzipped</t>
+  </si>
+  <si>
+    <t>Diff Compres hpack vs Gzipped</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,6 +85,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,13 +113,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -130,6 +150,30 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>JSON</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> size absolute comparison</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:view3D>
       <c:rotX val="15"/>
@@ -156,36 +200,59 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Sheet1!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Original JSON size (%)</c:v>
+                  <c:v>Original JSON size (bytes)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:f>Sheet1!$B$2:$F$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100</c:v>
+                  <c:v>52966</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>104370</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>233012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>493589</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1014099</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -196,7 +263,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$10</c:f>
+              <c:f>Sheet1!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -206,26 +273,49 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$F$10</c:f>
+              <c:f>Sheet1!$B$3:$F$3</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>62.912056791149041</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>77.27986969435662</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>77.386143202925169</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>77.472553075534506</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>76.534440917504114</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>33322</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80657</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180319</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>382396</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>776135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -236,36 +326,59 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sheet1!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gzipped</c:v>
+                  <c:v>Compress cjson</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$F$11</c:f>
+              <c:f>Sheet1!$B$4:$F$4</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9.9403390854510434</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.1489891731340425</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.8169193002935469</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.6935810968234701</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.2944525140050427</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>24899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>48605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108983</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>231760</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>471230</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -276,36 +389,59 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
+              <c:f>Sheet1!$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gzipped + Minimized</c:v>
+                  <c:v>Compress hpack</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$5:$F$5</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9.3852660197107589</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.8241831944045224</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.4680102312327259</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.3191805327914521</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.1497920814437244</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5727</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10781</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>49099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>99575</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -316,36 +452,248 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$13</c:f>
+              <c:f>Sheet1!$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gzipped + Compressed</c:v>
+                  <c:v>Gzipped</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:f>Sheet1!$B$6:$F$6</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4.8483933089151536</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.4121874101753376</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.0328395104114811</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.8604993223106678</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.7074289591055707</c:v>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2929</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5374</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11224</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23167</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43550</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gzipped + Minimized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2775</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5035</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10411</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21319</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42083</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gzipped + Compress cjson</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2568</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9397</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19055</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37597</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gzipped + Compress hpack</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$1:$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$9:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3493</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6981</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27358</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -361,21 +709,21 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="81724928"/>
-        <c:axId val="81726464"/>
+        <c:axId val="54922624"/>
+        <c:axId val="54982528"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="81724928"/>
+        <c:axId val="54922624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81726464"/>
+        <c:crossAx val="54982528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -383,7 +731,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81726464"/>
+        <c:axId val="54982528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -391,10 +739,10 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81724928"/>
+        <c:crossAx val="54922624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -456,36 +804,59 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2</c:f>
+              <c:f>Sheet1!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Original JSON size (bytes)</c:v>
+                  <c:v>Original JSON size (%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>Sheet1!$B$16:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>52966</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>104370</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>233012</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>493589</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1014099</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -496,7 +867,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -506,26 +877,49 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
+              <c:f>Sheet1!$B$17:$F$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>33322</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80657</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>180319</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>382396</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>776135</c:v>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>62.912056791149041</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>77.27986969435662</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>77.386143202925169</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.472553075534506</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.534440917504114</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -536,36 +930,59 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4</c:f>
+              <c:f>Sheet1!$A$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gzipped</c:v>
+                  <c:v>Compress cjson</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:f>Sheet1!$B$18:$F$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>5265</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5374</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>11224</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>23167</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43550</c:v>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>47.009402258052333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.569895563859347</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.771410914459345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46.954044761937567</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46.467849785869028</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -576,36 +993,59 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5</c:f>
+              <c:f>Sheet1!$A$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gzipped + Minimized</c:v>
+                  <c:v>Compress hpack</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$5:$F$5</c:f>
+              <c:f>Sheet1!$B$19:$F$19</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4971</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5035</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10411</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21319</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>42083</c:v>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10.812596760185778</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.329596627383347</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.9402605874375567</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.947344855740301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.8190610581412674</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,36 +1056,248 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6</c:f>
+              <c:f>Sheet1!$A$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Gzipped + Compressed</c:v>
+                  <c:v>Gzipped</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$6:$F$6</c:f>
+              <c:f>Sheet1!$B$20:$F$20</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>2568</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4605</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9397</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>19055</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>37597</c:v>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.5299626175282262</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1489891731340425</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8169193002935469</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6935810968234701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2944525140050427</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gzipped + Minimized</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$21:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.2392100592833142</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.8241831944045224</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4680102312327259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3191805327914521</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.1497920814437244</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gzipped + Compress cjson</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$22:$F$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.8483933089151536</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4121874101753376</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0328395104114811</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8604993223106678</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7074289591055707</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Gzipped + Compress hpack</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>json1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>json2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>json3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>json4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>json5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.7420231846845149</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3467471495640506</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9959830395001115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8359627139178549</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6977642222307683</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -661,12 +1313,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="97837056"/>
-        <c:axId val="97838592"/>
+        <c:axId val="93526656"/>
+        <c:axId val="93700480"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="97837056"/>
+        <c:axId val="93526656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -675,7 +1327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97838592"/>
+        <c:crossAx val="93700480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -683,7 +1335,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="97838592"/>
+        <c:axId val="93700480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,7 +1346,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="97837056"/>
+        <c:crossAx val="93526656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -720,20 +1372,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95251</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542924</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>180976</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>380999</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="13" name="Chart 12"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -750,20 +1402,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>100011</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvPr id="14" name="Chart 13"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1068,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,20 +1735,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1139,214 +1791,394 @@
         <v>776135</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>5265</v>
+        <v>24899</v>
       </c>
       <c r="C4">
-        <v>5374</v>
+        <v>48605</v>
       </c>
       <c r="D4">
-        <v>11224</v>
+        <v>108983</v>
       </c>
       <c r="E4">
-        <v>23167</v>
-      </c>
-      <c r="F4">
-        <v>43550</v>
+        <v>231760</v>
+      </c>
+      <c r="F4" s="2">
+        <v>471230</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5">
-        <v>4971</v>
+        <v>5727</v>
       </c>
       <c r="C5">
-        <v>5035</v>
+        <v>10781</v>
       </c>
       <c r="D5">
-        <v>10411</v>
+        <v>23162</v>
       </c>
       <c r="E5">
-        <v>21319</v>
+        <v>49099</v>
       </c>
       <c r="F5">
-        <v>42083</v>
+        <v>99575</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B6">
+        <v>2929</v>
+      </c>
+      <c r="C6">
+        <v>5374</v>
+      </c>
+      <c r="D6">
+        <v>11224</v>
+      </c>
+      <c r="E6">
+        <v>23167</v>
+      </c>
+      <c r="F6">
+        <v>43550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>2775</v>
+      </c>
+      <c r="C7">
+        <v>5035</v>
+      </c>
+      <c r="D7">
+        <v>10411</v>
+      </c>
+      <c r="E7">
+        <v>21319</v>
+      </c>
+      <c r="F7">
+        <v>42083</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
         <v>2568</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>4605</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <v>9397</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>19055</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>37597</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9">
+        <v>1982</v>
+      </c>
+      <c r="C9">
+        <v>3493</v>
+      </c>
+      <c r="D9">
+        <v>6981</v>
+      </c>
+      <c r="E9">
+        <v>13998</v>
+      </c>
+      <c r="F9">
+        <v>27358</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16">
         <f>B2/B2*100</f>
         <v>100</v>
       </c>
-      <c r="C9">
+      <c r="C16">
         <f>C2/C2*100</f>
         <v>100</v>
       </c>
-      <c r="D9">
+      <c r="D16">
         <f>D2/D2*100</f>
         <v>100</v>
       </c>
-      <c r="E9">
+      <c r="E16">
         <f>E2/E2*100</f>
         <v>100</v>
       </c>
-      <c r="F9">
+      <c r="F16">
         <f>F2/F2*100</f>
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B17" s="4">
         <f>B3/B2*100</f>
         <v>62.912056791149041</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C17" s="4">
         <f>C3/C2*100</f>
         <v>77.27986969435662</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D17" s="4">
         <f>D3/D2*100</f>
         <v>77.386143202925169</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E17" s="4">
         <f>E3/E2*100</f>
         <v>77.472553075534506</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F17" s="4">
         <f>F3/F2*100</f>
         <v>76.534440917504114</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4">
+        <f>B4/B2*100</f>
+        <v>47.009402258052333</v>
+      </c>
+      <c r="C18" s="4">
+        <f t="shared" ref="C18:F18" si="0">C4/C2*100</f>
+        <v>46.569895563859347</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>46.771410914459345</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>46.954044761937567</v>
+      </c>
+      <c r="F18" s="4">
+        <f t="shared" si="0"/>
+        <v>46.467849785869028</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4">
+        <f>B5/B2*100</f>
+        <v>10.812596760185778</v>
+      </c>
+      <c r="C19" s="4">
+        <f t="shared" ref="C19:E19" si="1">C5/C2*100</f>
+        <v>10.329596627383347</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="1"/>
+        <v>9.9402605874375567</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="1"/>
+        <v>9.947344855740301</v>
+      </c>
+      <c r="F19" s="4">
+        <f>F5/F2*100</f>
+        <v>9.8190610581412674</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="3">
-        <f>B4/B2*100</f>
-        <v>9.9403390854510434</v>
-      </c>
-      <c r="C11" s="3">
-        <f>C4/C2*100</f>
+      <c r="B20" s="4">
+        <f>B6/B2*100</f>
+        <v>5.5299626175282262</v>
+      </c>
+      <c r="C20" s="4">
+        <f>C6/C2*100</f>
         <v>5.1489891731340425</v>
       </c>
-      <c r="D11" s="3">
-        <f>D4/D2*100</f>
+      <c r="D20" s="4">
+        <f>D6/D2*100</f>
         <v>4.8169193002935469</v>
       </c>
-      <c r="E11" s="3">
-        <f>E4/E2*100</f>
+      <c r="E20" s="4">
+        <f>E6/E2*100</f>
         <v>4.6935810968234701</v>
       </c>
-      <c r="F11" s="3">
-        <f>F4/F2*100</f>
+      <c r="F20" s="4">
+        <f>F6/F2*100</f>
         <v>4.2944525140050427</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="3">
-        <f>B5/B2*100</f>
-        <v>9.3852660197107589</v>
-      </c>
-      <c r="C12" s="3">
-        <f>C5/C2*100</f>
+      <c r="B21" s="4">
+        <f>B7/B2*100</f>
+        <v>5.2392100592833142</v>
+      </c>
+      <c r="C21" s="4">
+        <f>C7/C2*100</f>
         <v>4.8241831944045224</v>
       </c>
-      <c r="D12" s="3">
-        <f>D5/D2*100</f>
+      <c r="D21" s="4">
+        <f>D7/D2*100</f>
         <v>4.4680102312327259</v>
       </c>
-      <c r="E12" s="3">
-        <f>E5/E2*100</f>
+      <c r="E21" s="4">
+        <f>E7/E2*100</f>
         <v>4.3191805327914521</v>
       </c>
-      <c r="F12" s="3">
-        <f>F5/F2*100</f>
+      <c r="F21" s="4">
+        <f>F7/F2*100</f>
         <v>4.1497920814437244</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
-        <f>B6/B2*100</f>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="4">
+        <f>B8/B2*100</f>
         <v>4.8483933089151536</v>
       </c>
-      <c r="C13" s="3">
-        <f t="shared" ref="C13:F13" si="0">C6/C2*100</f>
+      <c r="C22" s="4">
+        <f>C8/C2*100</f>
         <v>4.4121874101753376</v>
       </c>
-      <c r="D13" s="3">
-        <f t="shared" si="0"/>
+      <c r="D22" s="4">
+        <f>D8/D2*100</f>
         <v>4.0328395104114811</v>
       </c>
-      <c r="E13" s="3">
-        <f t="shared" si="0"/>
+      <c r="E22" s="4">
+        <f>E8/E2*100</f>
         <v>3.8604993223106678</v>
       </c>
-      <c r="F13" s="3">
-        <f t="shared" si="0"/>
+      <c r="F22" s="4">
+        <f>F8/F2*100</f>
         <v>3.7074289591055707</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="3">
-        <f>B12-B13</f>
-        <v>4.5368727107956053</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" ref="C14:F14" si="1">C12-C13</f>
-        <v>0.41199578422918481</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" si="1"/>
-        <v>0.43517072082124475</v>
-      </c>
-      <c r="E14" s="3">
-        <f t="shared" si="1"/>
-        <v>0.45868121048078425</v>
-      </c>
-      <c r="F14" s="3">
-        <f t="shared" si="1"/>
-        <v>0.44236312233815367</v>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="4">
+        <f>B9/B2*100</f>
+        <v>3.7420231846845149</v>
+      </c>
+      <c r="C23" s="4">
+        <f t="shared" ref="C23:F23" si="2">C9/C2*100</f>
+        <v>3.3467471495640506</v>
+      </c>
+      <c r="D23" s="4">
+        <f t="shared" si="2"/>
+        <v>2.9959830395001115</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="2"/>
+        <v>2.8359627139178549</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" si="2"/>
+        <v>2.6977642222307683</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="5">
+        <f>B20-B22</f>
+        <v>0.68156930861307252</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" ref="C24:F24" si="3">C20-C22</f>
+        <v>0.73680176295870492</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="3"/>
+        <v>0.78407978988206573</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" si="3"/>
+        <v>0.8330817745128023</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="3"/>
+        <v>0.587023554899472</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="5">
+        <f>B20-B23</f>
+        <v>1.7879394328437113</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" ref="C25:F25" si="4">C20-C23</f>
+        <v>1.8022420235699919</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="4"/>
+        <v>1.8209362607934354</v>
+      </c>
+      <c r="E25" s="5">
+        <f t="shared" si="4"/>
+        <v>1.8576183829056152</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="4"/>
+        <v>1.5966882917742744</v>
       </c>
     </row>
   </sheetData>

</xml_diff>